<commit_message>
Updated Memorylab for Fall 2024
</commit_message>
<xml_diff>
--- a/classic-labs/MemoryLab/1248/starter-code/CacheCharts.xlsx
+++ b/classic-labs/MemoryLab/1248/starter-code/CacheCharts.xlsx
@@ -1,26 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cabohn/textbook/labs/classic-labs/MemoryLab/new-hardware/starter-code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cbohn2/courses/textbook/labs/classic-labs/MemoryLab/1248/starter-code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5455063C-C764-8A43-A72A-C267F89282B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080B5932-496B-4346-A119-F08DAEA62367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="500" windowWidth="32540" windowHeight="20500" activeTab="4" xr2:uid="{C93E0F98-7BD9-504A-8311-46AFA0E4279F}"/>
+    <workbookView xWindow="1060" yWindow="760" windowWidth="32540" windowHeight="20500" activeTab="2" xr2:uid="{C93E0F98-7BD9-504A-8311-46AFA0E4279F}"/>
   </bookViews>
   <sheets>
     <sheet name="Cache Size" sheetId="2" r:id="rId1"/>
     <sheet name="Cache Line Size infer by time" sheetId="3" r:id="rId2"/>
-    <sheet name="Cache Line Size infer by hits" sheetId="5" r:id="rId3"/>
-    <sheet name="Data" sheetId="1" r:id="rId4"/>
-    <sheet name="Raw Data" sheetId="4" r:id="rId5"/>
+    <sheet name="Data" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Data!$G$2:$G$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Data!$G$2:$G$39</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,30 +40,8 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
   <si>
     <t>CACHE SIZE</t>
   </si>
@@ -188,198 +164,6 @@
   </si>
   <si>
     <t>TIME (microseconds)</t>
-  </si>
-  <si>
-    <t>INCREMENT</t>
-  </si>
-  <si>
-    <t>HITS</t>
-  </si>
-  <si>
-    <t>MISSES</t>
-  </si>
-  <si>
-    <t>READS</t>
-  </si>
-  <si>
-    <t>1 byte</t>
-  </si>
-  <si>
-    <t>Time spent working with data when stride is 1 bytes: 54800 microseconds</t>
-  </si>
-  <si>
-    <t>CACHE LINE SIZE by time (menu option 3)</t>
-  </si>
-  <si>
-    <t>CACHE LINE SIZE by hit rate (menu option 4)</t>
-  </si>
-  <si>
-    <t>CACHE SIZE by time (menu option 2)</t>
-  </si>
-  <si>
-    <t>Time spent working with data when working set is 32 bytes: 2000 microseconds</t>
-  </si>
-  <si>
-    <t>Time spent working with data when working set is 24576 bytes: 2000 microseconds</t>
-  </si>
-  <si>
-    <t>Time spent working with data when stride is 2 bytes: 55000 microseconds</t>
-  </si>
-  <si>
-    <t>Time spent working with data when working set is 40 bytes: 3000 microseconds</t>
-  </si>
-  <si>
-    <t>Time spent working with data when working set is 48 bytes: 4000 microseconds</t>
-  </si>
-  <si>
-    <t>Time spent working with data when working set is 64 bytes: 5000 microseconds</t>
-  </si>
-  <si>
-    <t>Time spent working with data when working set is 80 bytes: 6000 microseconds</t>
-  </si>
-  <si>
-    <t>Time spent working with data when working set is 96 bytes: 7000 microseconds</t>
-  </si>
-  <si>
-    <t>Time spent working with data when working set is 128 bytes: 8000 microseconds</t>
-  </si>
-  <si>
-    <t>Time spent working with data when working set is 160 bytes: 9000 microseconds</t>
-  </si>
-  <si>
-    <t>Time spent working with data when working set is 192 bytes: 10000 microseconds</t>
-  </si>
-  <si>
-    <t>Time spent working with data when working set is 256 bytes: 11000 microseconds</t>
-  </si>
-  <si>
-    <t>Time spent working with data when working set is 320 bytes: 12000 microseconds</t>
-  </si>
-  <si>
-    <t>Time spent working with data when working set is 384 bytes: 13000 microseconds</t>
-  </si>
-  <si>
-    <t>Time spent working with data when working set is 640 bytes: 15000 microseconds</t>
-  </si>
-  <si>
-    <t>Time spent working with data when working set is 768 bytes: 14000 microseconds</t>
-  </si>
-  <si>
-    <t>Time spent working with data when working set is 1024 bytes: 13000 microseconds</t>
-  </si>
-  <si>
-    <t>Time spent working with data when working set is 1280 bytes: 12000 microseconds</t>
-  </si>
-  <si>
-    <t>Time spent working with data when working set is 1536 bytes: 11000 microseconds</t>
-  </si>
-  <si>
-    <t>Time spent working with data when working set is 2048 bytes: 10000 microseconds</t>
-  </si>
-  <si>
-    <t>Time spent working with data when working set is 2560 bytes: 9000 microseconds</t>
-  </si>
-  <si>
-    <t>Time spent working with data when working set is 3072 bytes: 8000 microseconds</t>
-  </si>
-  <si>
-    <t>Time spent working with data when working set is 4096 bytes: 7000 microseconds</t>
-  </si>
-  <si>
-    <t>Time spent working with data when working set is 5120 bytes: 6000 microseconds</t>
-  </si>
-  <si>
-    <t>Time spent working with data when working set is 6144 bytes: 7000 microseconds</t>
-  </si>
-  <si>
-    <t>Time spent working with data when working set is 8192 bytes: 8000 microseconds</t>
-  </si>
-  <si>
-    <t>Time spent working with data when working set is 10240 bytes: 6000 microseconds</t>
-  </si>
-  <si>
-    <t>Time spent working with data when working set is 12288 bytes: 5000 microseconds</t>
-  </si>
-  <si>
-    <t>Time spent working with data when working set is 16384 bytes: 3000 microseconds</t>
-  </si>
-  <si>
-    <t>Time spent working with data when working set is 20480 bytes: 4000 microseconds</t>
-  </si>
-  <si>
-    <t>Time spent working with data when working set is 32768 bytes: 3000 microseconds</t>
-  </si>
-  <si>
-    <t>Time spent working with data when working set is 40960 bytes: 4000 microseconds</t>
-  </si>
-  <si>
-    <t>Time spent working with data when working set is 49152 bytes: 5000 microseconds</t>
-  </si>
-  <si>
-    <t>Time spent working with data when working set is 65536 bytes: 6000 microseconds</t>
-  </si>
-  <si>
-    <t>Time spent working with data when stride is 4 bytes: 55200 microseconds</t>
-  </si>
-  <si>
-    <t>Time spent working with data when stride is 8 bytes: 55400 microseconds</t>
-  </si>
-  <si>
-    <t>Time spent working with data when stride is 16 bytes: 55600 microseconds</t>
-  </si>
-  <si>
-    <t>Time spent working with data when stride is 32 bytes: 55800 microseconds</t>
-  </si>
-  <si>
-    <t>Accessing element x, then element x+0, yielded 0 cache hits out of 256 reads</t>
-  </si>
-  <si>
-    <t>Accessing element x, then element x+1, yielded 16 cache hits out of 256 reads</t>
-  </si>
-  <si>
-    <t>Accessing element x, then element x+2, yielded 32 cache hits out of 256 reads</t>
-  </si>
-  <si>
-    <t>Accessing element x, then element x+3, yielded 48 cache hits out of 256 reads</t>
-  </si>
-  <si>
-    <t>Accessing element x, then element x+4, yielded 64 cache hits out of 256 reads</t>
-  </si>
-  <si>
-    <t>Accessing element x, then element x+5, yielded 80 cache hits out of 256 reads</t>
-  </si>
-  <si>
-    <t>Accessing element x, then element x+6, yielded 96 cache hits out of 256 reads</t>
-  </si>
-  <si>
-    <t>Accessing element x, then element x+7, yielded 112 cache hits out of 256 reads</t>
-  </si>
-  <si>
-    <t>Accessing element x, then element x+8, yielded 128 cache hits out of 256 reads</t>
-  </si>
-  <si>
-    <t>Accessing element x, then element x+9, yielded 144 cache hits out of 256 reads</t>
-  </si>
-  <si>
-    <t>Accessing element x, then element x+11, yielded 176 cache hits out of 256 reads</t>
-  </si>
-  <si>
-    <t>Accessing element x, then element x+10, yielded 160 cache hits out of 256 reads</t>
-  </si>
-  <si>
-    <t>Accessing element x, then element x+12, yielded 192 cache hits out of 256 reads</t>
-  </si>
-  <si>
-    <t>Accessing element x, then element x+13, yielded 208 cache hits out of 256 reads</t>
-  </si>
-  <si>
-    <t>Accessing element x, then element x+14, yielded 224 cache hits out of 256 reads</t>
-  </si>
-  <si>
-    <t>Accessing element x, then element x+15, yielded 240 cache hits out of 256 reads</t>
-  </si>
-  <si>
-    <t>Time spent working with data when working set is 512 bytes: 14000 microseconds</t>
   </si>
 </sst>
 </file>
@@ -401,10 +185,10 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF21FF06"/>
-      <name val="Menlo"/>
+      <sz val="8"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -427,13 +211,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1171,53 +954,71 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Data!$A$40:$A$45</c:f>
+              <c:f>Data!$A$40:$A$48</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>1 byte</c:v>
+                  <c:v>2 bytes</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2 bytes</c:v>
+                  <c:v>4 bytes</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4 bytes</c:v>
+                  <c:v>8 bytes</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8 bytes</c:v>
+                  <c:v>16 bytes</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16 bytes</c:v>
+                  <c:v>32 bytes</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32 bytes</c:v>
+                  <c:v>64 bytes</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128 bytes</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>256 bytes</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>512 bytes</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$B$40:$B$45</c:f>
+              <c:f>Data!$B$40:$B$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>54800</c:v>
+                  <c:v>55000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>55000</c:v>
+                  <c:v>55200</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55200</c:v>
+                  <c:v>55400</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>55400</c:v>
+                  <c:v>55600</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>55600</c:v>
+                  <c:v>55800</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>55800</c:v>
+                  <c:v>56000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>56200</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>56400</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>56600</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1512,632 +1313,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:sysClr>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>Inference of Cache Line Size</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="stacked"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Data!$B$49</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>HITS</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>Data!$A$50:$A$65</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>15</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Data!$B$50:$B$65</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>96</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>112</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>144</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>160</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>176</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>192</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>208</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>224</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>240</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E5AC-FB41-A0FB-B84780F64EDC}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Data!$C$49</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>MISSES</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>Data!$A$50:$A$65</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>15</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Data!$C$50:$C$65</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>240</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>224</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>208</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>192</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>176</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>160</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>144</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>112</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>96</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-E5AC-FB41-A0FB-B84780F64EDC}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:overlap val="100"/>
-        <c:axId val="1685887119"/>
-        <c:axId val="1416430079"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="1685887119"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Read</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Increment</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1416430079"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1416430079"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="cross"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1685887119"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-        <c:majorUnit val="64"/>
-        <c:minorUnit val="16"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="l"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-</c:chartSpace>
-</file>
-
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2218,46 +1393,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -3290,516 +2425,11 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{3BD96459-FB1C-7448-AA1A-BA3878C2493A}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="155" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="161" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3810,18 +2440,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{AE3E37E2-CA34-CF48-8A96-A85832C04EAA}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="155" workbookViewId="0" zoomToFit="1"/>
-  </sheetViews>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</chartsheet>
-</file>
-
-<file path=xl/chartsheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{0E8E3D47-575E-1B4E-9347-3619AB69F859}">
-  <sheetPr/>
-  <sheetViews>
-    <sheetView zoomScale="155" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="161" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3832,7 +2451,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8676968" cy="6292645"/>
+    <xdr:ext cx="8684907" cy="6294783"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -3865,46 +2484,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8676968" cy="6292645"/>
+    <xdr:ext cx="8684907" cy="6294783"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{088C4C06-455C-1E43-9813-2496DA855938}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks noGrp="1"/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:absoluteAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:absoluteAnchor>
-    <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8676968" cy="6292645"/>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD7754B9-3B5A-FC60-6E8E-CC3F51E4036B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4224,10 +2810,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DA063B1-BC06-DD46-BF81-9C28C7BAF327}">
-  <dimension ref="A1:I65"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4241,7 +2827,6 @@
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
@@ -4249,8 +2834,7 @@
       <c r="A2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" cm="1">
-        <f t="array" ref="B2">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A2, " "),,12))</f>
+      <c r="B2">
         <v>2000</v>
       </c>
       <c r="I2" s="1"/>
@@ -4259,8 +2843,7 @@
       <c r="A3" t="s">
         <v>36</v>
       </c>
-      <c r="B3" cm="1">
-        <f t="array" ref="B3">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A3, " "),,12))</f>
+      <c r="B3">
         <v>3000</v>
       </c>
       <c r="I3" s="1"/>
@@ -4269,8 +2852,7 @@
       <c r="A4" t="s">
         <v>37</v>
       </c>
-      <c r="B4" cm="1">
-        <f t="array" ref="B4">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A4, " "),,12))</f>
+      <c r="B4">
         <v>4000</v>
       </c>
       <c r="I4" s="1"/>
@@ -4279,8 +2861,7 @@
       <c r="A5" t="s">
         <v>26</v>
       </c>
-      <c r="B5" cm="1">
-        <f t="array" ref="B5">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A5, " "),,12))</f>
+      <c r="B5">
         <v>5000</v>
       </c>
       <c r="I5" s="1"/>
@@ -4289,8 +2870,7 @@
       <c r="A6" t="s">
         <v>38</v>
       </c>
-      <c r="B6" cm="1">
-        <f t="array" ref="B6">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A6, " "),,12))</f>
+      <c r="B6">
         <v>6000</v>
       </c>
       <c r="I6" s="1"/>
@@ -4299,8 +2879,7 @@
       <c r="A7" t="s">
         <v>39</v>
       </c>
-      <c r="B7" cm="1">
-        <f t="array" ref="B7">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A7, " "),,12))</f>
+      <c r="B7">
         <v>7000</v>
       </c>
       <c r="I7" s="1"/>
@@ -4309,8 +2888,7 @@
       <c r="A8" t="s">
         <v>1</v>
       </c>
-      <c r="B8" cm="1">
-        <f t="array" ref="B8">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A8, " "),,12))</f>
+      <c r="B8">
         <v>8000</v>
       </c>
       <c r="I8" s="1"/>
@@ -4319,8 +2897,7 @@
       <c r="A9" t="s">
         <v>27</v>
       </c>
-      <c r="B9" cm="1">
-        <f t="array" ref="B9">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A9, " "),,12))</f>
+      <c r="B9">
         <v>9000</v>
       </c>
       <c r="I9" s="1"/>
@@ -4329,8 +2906,7 @@
       <c r="A10" t="s">
         <v>2</v>
       </c>
-      <c r="B10" cm="1">
-        <f t="array" ref="B10">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A10, " "),,12))</f>
+      <c r="B10">
         <v>10000</v>
       </c>
       <c r="I10" s="1"/>
@@ -4339,8 +2915,7 @@
       <c r="A11" t="s">
         <v>3</v>
       </c>
-      <c r="B11" cm="1">
-        <f t="array" ref="B11">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A11, " "),,12))</f>
+      <c r="B11">
         <v>11000</v>
       </c>
       <c r="I11" s="1"/>
@@ -4349,8 +2924,7 @@
       <c r="A12" t="s">
         <v>28</v>
       </c>
-      <c r="B12" cm="1">
-        <f t="array" ref="B12">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A12, " "),,12))</f>
+      <c r="B12">
         <v>12000</v>
       </c>
       <c r="I12" s="1"/>
@@ -4359,8 +2933,7 @@
       <c r="A13" t="s">
         <v>4</v>
       </c>
-      <c r="B13" cm="1">
-        <f t="array" ref="B13">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A13, " "),,12))</f>
+      <c r="B13">
         <v>13000</v>
       </c>
       <c r="I13" s="1"/>
@@ -4369,8 +2942,7 @@
       <c r="A14" t="s">
         <v>5</v>
       </c>
-      <c r="B14" cm="1">
-        <f t="array" ref="B14">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A14, " "),,12))</f>
+      <c r="B14">
         <v>14000</v>
       </c>
       <c r="I14" s="1"/>
@@ -4379,8 +2951,7 @@
       <c r="A15" t="s">
         <v>29</v>
       </c>
-      <c r="B15" cm="1">
-        <f t="array" ref="B15">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A15, " "),,12))</f>
+      <c r="B15">
         <v>15000</v>
       </c>
       <c r="I15" s="1"/>
@@ -4389,8 +2960,7 @@
       <c r="A16" t="s">
         <v>6</v>
       </c>
-      <c r="B16" cm="1">
-        <f t="array" ref="B16">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A16, " "),,12))</f>
+      <c r="B16">
         <v>14000</v>
       </c>
       <c r="I16" s="1"/>
@@ -4399,8 +2969,7 @@
       <c r="A17" t="s">
         <v>7</v>
       </c>
-      <c r="B17" cm="1">
-        <f t="array" ref="B17">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A17, " "),,12))</f>
+      <c r="B17">
         <v>13000</v>
       </c>
       <c r="I17" s="1"/>
@@ -4409,8 +2978,7 @@
       <c r="A18" t="s">
         <v>30</v>
       </c>
-      <c r="B18" cm="1">
-        <f t="array" ref="B18">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A18, " "),,12))</f>
+      <c r="B18">
         <v>12000</v>
       </c>
       <c r="I18" s="1"/>
@@ -4419,8 +2987,7 @@
       <c r="A19" t="s">
         <v>8</v>
       </c>
-      <c r="B19" cm="1">
-        <f t="array" ref="B19">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A19, " "),,12))</f>
+      <c r="B19">
         <v>11000</v>
       </c>
       <c r="I19" s="1"/>
@@ -4429,8 +2996,7 @@
       <c r="A20" t="s">
         <v>9</v>
       </c>
-      <c r="B20" cm="1">
-        <f t="array" ref="B20">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A20, " "),,12))</f>
+      <c r="B20">
         <v>10000</v>
       </c>
       <c r="I20" s="1"/>
@@ -4439,8 +3005,7 @@
       <c r="A21" t="s">
         <v>31</v>
       </c>
-      <c r="B21" cm="1">
-        <f t="array" ref="B21">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A21, " "),,12))</f>
+      <c r="B21">
         <v>9000</v>
       </c>
       <c r="I21" s="1"/>
@@ -4449,8 +3014,7 @@
       <c r="A22" t="s">
         <v>10</v>
       </c>
-      <c r="B22" cm="1">
-        <f t="array" ref="B22">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A22, " "),,12))</f>
+      <c r="B22">
         <v>8000</v>
       </c>
       <c r="I22" s="1"/>
@@ -4459,8 +3023,7 @@
       <c r="A23" t="s">
         <v>11</v>
       </c>
-      <c r="B23" cm="1">
-        <f t="array" ref="B23">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A23, " "),,12))</f>
+      <c r="B23">
         <v>7000</v>
       </c>
       <c r="I23" s="1"/>
@@ -4469,8 +3032,7 @@
       <c r="A24" t="s">
         <v>32</v>
       </c>
-      <c r="B24" cm="1">
-        <f t="array" ref="B24">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A24, " "),,12))</f>
+      <c r="B24">
         <v>6000</v>
       </c>
       <c r="I24" s="1"/>
@@ -4479,8 +3041,7 @@
       <c r="A25" t="s">
         <v>12</v>
       </c>
-      <c r="B25" cm="1">
-        <f t="array" ref="B25">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A25, " "),,12))</f>
+      <c r="B25">
         <v>7000</v>
       </c>
       <c r="I25" s="1"/>
@@ -4489,8 +3050,7 @@
       <c r="A26" t="s">
         <v>13</v>
       </c>
-      <c r="B26" cm="1">
-        <f t="array" ref="B26">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A26, " "),,12))</f>
+      <c r="B26">
         <v>8000</v>
       </c>
       <c r="I26" s="1"/>
@@ -4499,8 +3059,7 @@
       <c r="A27" t="s">
         <v>33</v>
       </c>
-      <c r="B27" cm="1">
-        <f t="array" ref="B27">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A27, " "),,12))</f>
+      <c r="B27">
         <v>6000</v>
       </c>
       <c r="I27" s="1"/>
@@ -4509,8 +3068,7 @@
       <c r="A28" t="s">
         <v>14</v>
       </c>
-      <c r="B28" cm="1">
-        <f t="array" ref="B28">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A28, " "),,12))</f>
+      <c r="B28">
         <v>5000</v>
       </c>
       <c r="I28" s="1"/>
@@ -4519,8 +3077,7 @@
       <c r="A29" t="s">
         <v>15</v>
       </c>
-      <c r="B29" cm="1">
-        <f t="array" ref="B29">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A29, " "),,12))</f>
+      <c r="B29">
         <v>3000</v>
       </c>
       <c r="I29" s="1"/>
@@ -4529,8 +3086,7 @@
       <c r="A30" t="s">
         <v>34</v>
       </c>
-      <c r="B30" cm="1">
-        <f t="array" ref="B30">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A30, " "),,12))</f>
+      <c r="B30">
         <v>4000</v>
       </c>
       <c r="I30" s="1"/>
@@ -4539,8 +3095,7 @@
       <c r="A31" t="s">
         <v>16</v>
       </c>
-      <c r="B31" cm="1">
-        <f t="array" ref="B31">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A31, " "),,12))</f>
+      <c r="B31">
         <v>2000</v>
       </c>
       <c r="I31" s="1"/>
@@ -4549,8 +3104,7 @@
       <c r="A32" t="s">
         <v>17</v>
       </c>
-      <c r="B32" cm="1">
-        <f t="array" ref="B32">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A32, " "),,12))</f>
+      <c r="B32">
         <v>3000</v>
       </c>
       <c r="I32" s="1"/>
@@ -4559,8 +3113,7 @@
       <c r="A33" t="s">
         <v>35</v>
       </c>
-      <c r="B33" cm="1">
-        <f t="array" ref="B33">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A33, " "),,12))</f>
+      <c r="B33">
         <v>4000</v>
       </c>
       <c r="I33" s="1"/>
@@ -4569,8 +3122,7 @@
       <c r="A34" t="s">
         <v>18</v>
       </c>
-      <c r="B34" cm="1">
-        <f t="array" ref="B34">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A34, " "),,12))</f>
+      <c r="B34">
         <v>5000</v>
       </c>
       <c r="I34" s="1"/>
@@ -4579,8 +3131,7 @@
       <c r="A35" t="s">
         <v>19</v>
       </c>
-      <c r="B35" cm="1">
-        <f t="array" ref="B35">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A35, " "),,12))</f>
+      <c r="B35">
         <v>6000</v>
       </c>
       <c r="I35" s="1"/>
@@ -4605,691 +3156,78 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>45</v>
-      </c>
-      <c r="B40" cm="1">
-        <f t="array" ref="B40">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A40, " "),,11))</f>
-        <v>54800</v>
+        <v>21</v>
+      </c>
+      <c r="B40">
+        <v>55000</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>21</v>
-      </c>
-      <c r="B41" cm="1">
-        <f t="array" ref="B41">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A41, " "),,11))</f>
-        <v>55000</v>
+        <v>22</v>
+      </c>
+      <c r="B41">
+        <v>55200</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>22</v>
-      </c>
-      <c r="B42" cm="1">
-        <f t="array" ref="B42">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A42, " "),,11))</f>
-        <v>55200</v>
+        <v>23</v>
+      </c>
+      <c r="B42">
+        <v>55400</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>23</v>
-      </c>
-      <c r="B43" cm="1">
-        <f t="array" ref="B43">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A43, " "),,11))</f>
-        <v>55400</v>
+        <v>24</v>
+      </c>
+      <c r="B43">
+        <v>55600</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>24</v>
-      </c>
-      <c r="B44" cm="1">
-        <f t="array" ref="B44">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A44, " "),,11))</f>
-        <v>55600</v>
+        <v>25</v>
+      </c>
+      <c r="B44">
+        <v>55800</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>25</v>
-      </c>
-      <c r="B45" cm="1">
-        <f t="array" ref="B45">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A45, " "),,11))</f>
-        <v>55800</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>41</v>
-      </c>
-      <c r="B49" t="s">
-        <v>42</v>
-      </c>
-      <c r="C49" t="s">
-        <v>43</v>
-      </c>
-      <c r="D49" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50">
-        <v>0</v>
-      </c>
-      <c r="B50" cm="1">
-        <f t="array" ref="B50">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A50, " "),,8))</f>
-        <v>0</v>
-      </c>
-      <c r="C50">
-        <f>D50-B50</f>
-        <v>256</v>
-      </c>
-      <c r="D50" cm="1">
-        <f t="array" ref="D50">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A50, " "),,13))</f>
-        <v>256</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51">
-        <f>A50+1</f>
+        <v>26</v>
+      </c>
+      <c r="B45">
+        <v>56000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>1</v>
       </c>
-      <c r="B51" cm="1">
-        <f t="array" ref="B51">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A51, " "),,8))</f>
-        <v>16</v>
-      </c>
-      <c r="C51">
-        <f>D51-B51</f>
-        <v>240</v>
-      </c>
-      <c r="D51" cm="1">
-        <f t="array" ref="D51">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A51, " "),,13))</f>
-        <v>256</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52">
-        <f t="shared" ref="A52:A65" si="0">A51+1</f>
-        <v>2</v>
-      </c>
-      <c r="B52" cm="1">
-        <f t="array" ref="B52">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A52, " "),,8))</f>
-        <v>32</v>
-      </c>
-      <c r="C52">
-        <f t="shared" ref="C52:C65" si="1">D52-B52</f>
-        <v>224</v>
-      </c>
-      <c r="D52" cm="1">
-        <f t="array" ref="D52">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A52, " "),,13))</f>
-        <v>256</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53">
-        <f t="shared" si="0"/>
+      <c r="B46">
+        <v>56200</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>3</v>
       </c>
-      <c r="B53" cm="1">
-        <f t="array" ref="B53">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A53, " "),,8))</f>
-        <v>48</v>
-      </c>
-      <c r="C53">
-        <f t="shared" si="1"/>
-        <v>208</v>
-      </c>
-      <c r="D53" cm="1">
-        <f t="array" ref="D53">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A53, " "),,13))</f>
-        <v>256</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B54" cm="1">
-        <f t="array" ref="B54">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A54, " "),,8))</f>
-        <v>64</v>
-      </c>
-      <c r="C54">
-        <f t="shared" si="1"/>
-        <v>192</v>
-      </c>
-      <c r="D54" cm="1">
-        <f t="array" ref="D54">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A54, " "),,13))</f>
-        <v>256</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55">
-        <f t="shared" si="0"/>
+      <c r="B47">
+        <v>56400</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>5</v>
       </c>
-      <c r="B55" cm="1">
-        <f t="array" ref="B55">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A55, " "),,8))</f>
-        <v>80</v>
-      </c>
-      <c r="C55">
-        <f t="shared" si="1"/>
-        <v>176</v>
-      </c>
-      <c r="D55" cm="1">
-        <f t="array" ref="D55">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A55, " "),,13))</f>
-        <v>256</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B56" cm="1">
-        <f t="array" ref="B56">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A56, " "),,8))</f>
-        <v>96</v>
-      </c>
-      <c r="C56">
-        <f t="shared" si="1"/>
-        <v>160</v>
-      </c>
-      <c r="D56" cm="1">
-        <f t="array" ref="D56">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A56, " "),,13))</f>
-        <v>256</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B57" cm="1">
-        <f t="array" ref="B57">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A57, " "),,8))</f>
-        <v>112</v>
-      </c>
-      <c r="C57">
-        <f t="shared" si="1"/>
-        <v>144</v>
-      </c>
-      <c r="D57" cm="1">
-        <f t="array" ref="D57">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A57, " "),,13))</f>
-        <v>256</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B58" cm="1">
-        <f t="array" ref="B58">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A58, " "),,8))</f>
-        <v>128</v>
-      </c>
-      <c r="C58">
-        <f t="shared" si="1"/>
-        <v>128</v>
-      </c>
-      <c r="D58" cm="1">
-        <f t="array" ref="D58">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A58, " "),,13))</f>
-        <v>256</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B59" cm="1">
-        <f t="array" ref="B59">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A59, " "),,8))</f>
-        <v>144</v>
-      </c>
-      <c r="C59">
-        <f t="shared" si="1"/>
-        <v>112</v>
-      </c>
-      <c r="D59" cm="1">
-        <f t="array" ref="D59">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A59, " "),,13))</f>
-        <v>256</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B60" cm="1">
-        <f t="array" ref="B60">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A60, " "),,8))</f>
-        <v>160</v>
-      </c>
-      <c r="C60">
-        <f t="shared" si="1"/>
-        <v>96</v>
-      </c>
-      <c r="D60" cm="1">
-        <f t="array" ref="D60">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A60, " "),,13))</f>
-        <v>256</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B61" cm="1">
-        <f t="array" ref="B61">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A61, " "),,8))</f>
-        <v>176</v>
-      </c>
-      <c r="C61">
-        <f t="shared" si="1"/>
-        <v>80</v>
-      </c>
-      <c r="D61" cm="1">
-        <f t="array" ref="D61">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A61, " "),,13))</f>
-        <v>256</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="B62" cm="1">
-        <f t="array" ref="B62">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A62, " "),,8))</f>
-        <v>192</v>
-      </c>
-      <c r="C62">
-        <f t="shared" si="1"/>
-        <v>64</v>
-      </c>
-      <c r="D62" cm="1">
-        <f t="array" ref="D62">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A62, " "),,13))</f>
-        <v>256</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="B63" cm="1">
-        <f t="array" ref="B63">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A63, " "),,8))</f>
-        <v>208</v>
-      </c>
-      <c r="C63">
-        <f t="shared" si="1"/>
-        <v>48</v>
-      </c>
-      <c r="D63" cm="1">
-        <f t="array" ref="D63">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A63, " "),,13))</f>
-        <v>256</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="B64" cm="1">
-        <f t="array" ref="B64">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A64, " "),,8))</f>
-        <v>224</v>
-      </c>
-      <c r="C64">
-        <f t="shared" si="1"/>
-        <v>32</v>
-      </c>
-      <c r="D64" cm="1">
-        <f t="array" ref="D64">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A64, " "),,13))</f>
-        <v>256</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="B65" cm="1">
-        <f t="array" ref="B65">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A65, " "),,8))</f>
-        <v>240</v>
-      </c>
-      <c r="C65">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="D65" cm="1">
-        <f t="array" ref="D65">VALUE(INDEX(_xlfn.TEXTSPLIT('Raw Data'!A65, " "),,13))</f>
-        <v>256</v>
+      <c r="B48">
+        <v>56600</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB66E5A9-00E7-224D-B37E-C4BDE8B14A62}">
-  <dimension ref="A1:A65"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="11" max="11" width="11" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="1"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="1"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="1"/>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" s="3"/>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47" s="3"/>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48" s="1"/>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A55" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A56" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A57" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A58" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A59" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A60" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A61" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A62" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A63" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A64" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A65" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>